<commit_message>
update style, add imgs
</commit_message>
<xml_diff>
--- a/data_excel/tags.xlsx
+++ b/data_excel/tags.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jay/xidev/signs-db/data_excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jay/xidev/kanban-corpus/data_excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B07A0BA1-548F-8D4C-9025-A303FD66D897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC8DCB97-0798-A248-B720-04AC27350A45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14360" yWindow="500" windowWidth="24040" windowHeight="17360" xr2:uid="{1951D371-7A8D-D346-B651-736256765602}"/>
+    <workbookView xWindow="14620" yWindow="500" windowWidth="23780" windowHeight="17360" xr2:uid="{1951D371-7A8D-D346-B651-736256765602}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="124">
   <si>
     <t>img</t>
     <phoneticPr fontId="1"/>
@@ -162,22 +162,7 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>天候により
-床すべり注意</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ジェフグルメカード
-加盟店</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>ロゴマーク|全国共通お食事券ジェフグルメカード加盟店</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ペット
-ご遠慮下さい</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -204,11 +189,6 @@
     <rPh sb="5" eb="6">
       <t xml:space="preserve">イヌ </t>
     </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>未成年・運転者
-飲酒禁止</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -471,10 +451,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>ja|en|zh|ko</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>ja</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -626,13 +602,6 @@
   </si>
   <si>
     <t>IMG_6329.JPG</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>日東CS
-1F OR・レストラン 用
-清掃中
-足元にご注意！</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -691,12 +660,449 @@
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>ジェフグルメカード加盟店</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>天候により 床すべり注意</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ペット ご遠慮下さい</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>未成年・運転者 飲酒禁止</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>清掃中
+足元にご注意！</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>IMG_9358.HEIC</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>自転車の自由通路への昇降（↓↑）はエレベーターをご利用ください</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>南北自由通路
+South-North Promenade
+大和西大寺駅
+Yamato-Saidaiji Station</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>エレベーター|人|自転車を押す人</t>
+    <rPh sb="7" eb="8">
+      <t xml:space="preserve">ヒト </t>
+    </rPh>
+    <rPh sb="9" eb="12">
+      <t xml:space="preserve">ジテンシャヲ </t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t xml:space="preserve">オスヒト </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>禁止事項 Prohibited activities</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>自転車走行
+Riding a bicycle</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>自転車駐輪
+Bicydle parking</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>バイク乗り入れ
+Riding a motorcycle</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>喫煙
+Smoking</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>歩きスマホ
+Using a smartphone while walking</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>不法投棄
+Illegal dumping</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>火器類の使用
+Use of fire</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>●他の通行者の迷惑になる行為
+●危険の恐れのある行為
+●ポール遊び・ローラースケート・スケートポード
+●通路の損傷および汚損
+●座り込み・寝泊り
+●ポスターの掲示・看板の設置
+●物品の配布・販売
+●集会・デモ・演説</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>防犯カメラ作動中
+Security Cameras in Operation</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>赤丸斜線|倒れる人|衝突|自転車に乗る人</t>
+    <rPh sb="10" eb="12">
+      <t xml:space="preserve">ショウトツ </t>
+    </rPh>
+    <rPh sb="13" eb="16">
+      <t xml:space="preserve">ジテンシャン </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>赤丸斜線|自転車</t>
+    <rPh sb="0" eb="1">
+      <t xml:space="preserve">アカマル </t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t xml:space="preserve">シャセン </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>赤丸斜線|バイク</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>赤丸斜線|スマホを持って歩く人</t>
+    <rPh sb="9" eb="10">
+      <t xml:space="preserve">モッテアルク </t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t xml:space="preserve">ヒト </t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t/>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>赤丸斜線|手|丸めた紙</t>
+    <rPh sb="5" eb="6">
+      <t>☚</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t xml:space="preserve">マルメタカミ </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>赤丸斜線|マッチ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>駐車禁止</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>IMG_8116.HEIC</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>IMG_7162.jpg</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>お願い！
+大変危険ですのでパーテンションをまたがないでください！</t>
+    <rPh sb="5" eb="7">
+      <t xml:space="preserve">タイヘン </t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t xml:space="preserve">キケン </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ロープ|貼紙</t>
+    <rPh sb="4" eb="6">
+      <t xml:space="preserve">ハリガミ </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>IMG_4856.HEIC</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>危院！！立入禁止
+Danger!! Off-limits
+危</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Microsoft JhengHei"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t>险</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>！！</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Microsoft JhengHei"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t>请</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>别</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Microsoft JhengHei"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t>进</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">入
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>위험하다</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">!! </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>출입금지</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>警官|手のひらをこちらへ向ける|No!と書かれた板</t>
+    <rPh sb="0" eb="2">
+      <t xml:space="preserve">ケイカン </t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t xml:space="preserve">テノヒラヲ </t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t xml:space="preserve">イタ </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ヘルメットを被った人|手のひらをこちらへ向ける|赤四角バツ</t>
+    <rPh sb="6" eb="7">
+      <t xml:space="preserve">カブッタヒト </t>
+    </rPh>
+    <rPh sb="24" eb="27">
+      <t xml:space="preserve">アカシカク </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ja|en|zh|ko|multi</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>IMG_4583.HEIC</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>駐輪禁止
+駐輪場に止めること。
+基礎工学部長</t>
+    <rPh sb="0" eb="1">
+      <t xml:space="preserve">チュウリンキンシ </t>
+    </rPh>
+    <rPh sb="5" eb="8">
+      <t xml:space="preserve">チュウリンジョウニ </t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t xml:space="preserve">トメルコト </t>
+    </rPh>
+    <rPh sb="16" eb="22">
+      <t xml:space="preserve">キソコウガクブチョウ </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>IMG_4324_2.heic</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>時間帯禁煙
+平日11:30～14:00 禁煙
+平日14:00~18:00 喫煙
+平日18:00~最終 禁煙
+土・日・祝日は、すべての時間が禁煙になります。
+ご協力お願いします。</t>
+    <rPh sb="0" eb="3">
+      <t xml:space="preserve">ジカンタイ </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>赤丸斜線|タバコ|時計</t>
+    <rPh sb="0" eb="1">
+      <t xml:space="preserve">アカマル </t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t xml:space="preserve">トケイ </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ご注文が決まればレジ前カウンターでご注文して下さい。（料金は先払いになります。）
+お水のおかわりはセルフサービスになります。自由にどうぞ。</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>IMG_4324.heic</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>かぶりつき厳禁！
+生煎包は、いきなりほおばろうとすると、熱いスープが飛び出し大変危険です。
+生煎包をレンゲに乗せ箸や口で穴をあけて、やけどに気をつけながらスープを楽しみください。
+その後、残った肉と皮をお召し上がり下さい。
+味はしっかりついています。先ずは何も付けずにそのままの味をお楽しみ下さい。その後、お好みで黒酢を付けて下さい。黒酢を付けるとさっぱと頂けます。</t>
+    <rPh sb="5" eb="7">
+      <t>💰</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>オレンジ三角|火|赤丸斜線|液体が飛び出す生煎包|レンゲにのった生煎包|皿の上に並んだ生煎包</t>
+    <rPh sb="4" eb="6">
+      <t>‣</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t xml:space="preserve">ヒ </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>IMG_4147.HEIC</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>南区は終日駐車禁止です。
+我々区分所有者の有料駐車場の出入口です。ここに駐車されますと車の出入が出来ません。
+不法駐車されますとレッカー車を要請します。
+道頓堀区分所有者管理組合</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>キケン
+携帯電話などを操作しながらホームを歩くのは大変危険です
+駅長</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>IMG_1689.HEIC</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>看板|黄ダイヤ|人|スマホ|電車|線路</t>
+    <rPh sb="0" eb="2">
+      <t xml:space="preserve">カンバン </t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>🌲</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t xml:space="preserve">ヒト </t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t xml:space="preserve">デンシャ </t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t xml:space="preserve">センロ </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -726,6 +1132,13 @@
       <name val="Malgun Gothic"/>
       <family val="2"/>
       <charset val="129"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Microsoft JhengHei"/>
+      <family val="2"/>
+      <charset val="128"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1094,9 +1507,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0244D4E8-F443-D54E-A975-960F8853E327}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="166" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="106" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
   <cols>
@@ -1123,567 +1538,987 @@
         <v>9</v>
       </c>
       <c r="F1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="147">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="42">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>80</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>4</v>
+        <v>81</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="105">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="84">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>80</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>82</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>83</v>
       </c>
       <c r="E3" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="F3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="84">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="21">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>80</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D4" t="s">
         <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="F4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="84">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="42">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>80</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>13</v>
+        <v>85</v>
       </c>
       <c r="D5" t="s">
+        <v>94</v>
+      </c>
+      <c r="E5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="42">
+      <c r="A6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D6" t="s">
+        <v>95</v>
+      </c>
+      <c r="E6" t="s">
+        <v>72</v>
+      </c>
+      <c r="F6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="42">
+      <c r="A7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7">
         <v>5</v>
       </c>
-      <c r="E5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="84">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="C7" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D7" t="s">
+        <v>96</v>
+      </c>
+      <c r="E7" t="s">
+        <v>72</v>
+      </c>
+      <c r="F7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="42">
+      <c r="A8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" t="s">
+        <v>72</v>
+      </c>
+      <c r="F8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="42">
+      <c r="A9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E9" t="s">
+        <v>72</v>
+      </c>
+      <c r="F9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="42">
+      <c r="A10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D10" t="s">
+        <v>98</v>
+      </c>
+      <c r="E10" t="s">
+        <v>72</v>
+      </c>
+      <c r="F10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="42">
+      <c r="A11" t="s">
+        <v>80</v>
+      </c>
+      <c r="B11">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D11" t="s">
+        <v>99</v>
+      </c>
+      <c r="E11" t="s">
+        <v>72</v>
+      </c>
+      <c r="F11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="168">
+      <c r="A12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D12" t="s">
         <v>5</v>
       </c>
-      <c r="E6" t="s">
-        <v>50</v>
-      </c>
-      <c r="F6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="21">
-      <c r="A7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" t="s">
-        <v>50</v>
-      </c>
-      <c r="F7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="21">
-      <c r="A8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" t="s">
-        <v>50</v>
-      </c>
-      <c r="F8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="42">
-      <c r="A9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9">
-        <v>2</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" t="s">
-        <v>50</v>
-      </c>
-      <c r="F9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="42">
-      <c r="A10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10">
-        <v>3</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" t="s">
-        <v>50</v>
-      </c>
-      <c r="F10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="42">
-      <c r="A11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11">
-        <v>4</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" t="s">
-        <v>50</v>
-      </c>
-      <c r="F11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="42">
-      <c r="A12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12">
+      <c r="E12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="42">
+      <c r="A13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13">
+        <v>11</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D13" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" t="s">
-        <v>25</v>
-      </c>
-      <c r="E12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="42">
-      <c r="A13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13">
-        <v>6</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" t="s">
-        <v>28</v>
-      </c>
       <c r="E13" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="F13" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="21">
-      <c r="A14" s="2" t="s">
-        <v>15</v>
+      <c r="A14" t="s">
+        <v>101</v>
       </c>
       <c r="B14">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>29</v>
+        <v>100</v>
       </c>
       <c r="D14" t="s">
-        <v>30</v>
+        <v>107</v>
       </c>
       <c r="E14" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="399">
-      <c r="A15" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="63">
+      <c r="A15" t="s">
+        <v>102</v>
       </c>
       <c r="B15">
         <v>0</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>32</v>
+        <v>103</v>
       </c>
       <c r="D15" t="s">
         <v>5</v>
       </c>
       <c r="E15" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F15" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="63">
-      <c r="A16" s="2" t="s">
-        <v>31</v>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="84">
+      <c r="A16" t="s">
+        <v>105</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>33</v>
+        <v>106</v>
       </c>
       <c r="D16" t="s">
-        <v>5</v>
+        <v>108</v>
       </c>
       <c r="E16" t="s">
-        <v>50</v>
+        <v>109</v>
       </c>
       <c r="F16" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="84">
-      <c r="A17" s="2" t="s">
-        <v>35</v>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="63">
+      <c r="A17" t="s">
+        <v>110</v>
       </c>
       <c r="B17">
         <v>0</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>36</v>
+        <v>111</v>
       </c>
       <c r="D17" t="s">
         <v>5</v>
       </c>
       <c r="E17" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F17" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="21">
-      <c r="A18" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="126">
+      <c r="A18" t="s">
+        <v>112</v>
       </c>
       <c r="B18">
         <v>0</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>37</v>
+        <v>113</v>
       </c>
       <c r="D18" t="s">
-        <v>39</v>
+        <v>114</v>
       </c>
       <c r="E18" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F18" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="126">
-      <c r="A19" s="2" t="s">
         <v>46</v>
       </c>
+    </row>
+    <row r="19" spans="1:6" ht="84">
+      <c r="A19" t="s">
+        <v>112</v>
+      </c>
       <c r="B19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>47</v>
+        <v>115</v>
       </c>
       <c r="D19" t="s">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="E19" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F19" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="42">
-      <c r="A20" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="189">
+      <c r="A20" t="s">
+        <v>116</v>
       </c>
       <c r="B20">
         <v>0</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>53</v>
+        <v>117</v>
       </c>
       <c r="D20" t="s">
-        <v>65</v>
+        <v>118</v>
       </c>
       <c r="E20" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F20" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="21">
-      <c r="A21" s="2" t="s">
-        <v>56</v>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="105">
+      <c r="A21" t="s">
+        <v>119</v>
       </c>
       <c r="B21">
         <v>0</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>55</v>
+        <v>120</v>
       </c>
       <c r="D21" t="s">
         <v>5</v>
       </c>
       <c r="E21" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F21" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="84">
-      <c r="A22" s="2" t="s">
-        <v>56</v>
+      <c r="A22" t="s">
+        <v>122</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>59</v>
+        <v>121</v>
       </c>
       <c r="D22" t="s">
-        <v>5</v>
+        <v>123</v>
       </c>
       <c r="E22" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F22" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="42">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="21">
       <c r="A23" s="2" t="s">
-        <v>61</v>
+        <v>34</v>
       </c>
       <c r="B23">
         <v>0</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="D23" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="E23" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F23" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="63">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="84">
       <c r="A24" s="2" t="s">
-        <v>63</v>
+        <v>31</v>
       </c>
       <c r="B24">
         <v>0</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>62</v>
+        <v>32</v>
       </c>
       <c r="D24" t="s">
         <v>5</v>
       </c>
       <c r="E24" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F24" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="126">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="399">
       <c r="A25" s="2" t="s">
-        <v>70</v>
+        <v>27</v>
       </c>
       <c r="B25">
         <v>0</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>64</v>
+        <v>28</v>
       </c>
       <c r="D25" t="s">
-        <v>66</v>
+        <v>5</v>
       </c>
       <c r="E25" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F25" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="63">
-      <c r="A26" t="s">
-        <v>69</v>
+      <c r="A26" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="B26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>67</v>
+        <v>29</v>
       </c>
       <c r="D26" t="s">
-        <v>68</v>
+        <v>5</v>
       </c>
       <c r="E26" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F26" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="84">
       <c r="A27" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" t="s">
+        <v>45</v>
+      </c>
+      <c r="F27" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="84">
+      <c r="A28" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" t="s">
+        <v>45</v>
+      </c>
+      <c r="F28" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="84">
+      <c r="A29" t="s">
+        <v>11</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" t="s">
+        <v>5</v>
+      </c>
+      <c r="E29" t="s">
+        <v>45</v>
+      </c>
+      <c r="F29" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="105">
+      <c r="A30" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" t="s">
+        <v>5</v>
+      </c>
+      <c r="E30" t="s">
+        <v>45</v>
+      </c>
+      <c r="F30" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="147">
+      <c r="A31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" t="s">
+        <v>5</v>
+      </c>
+      <c r="E31" t="s">
+        <v>45</v>
+      </c>
+      <c r="F31" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="105">
+      <c r="A32" t="s">
+        <v>73</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D32" t="s">
+        <v>67</v>
+      </c>
+      <c r="E32" t="s">
         <v>72</v>
       </c>
-      <c r="B27">
-        <v>0</v>
-      </c>
-      <c r="C27" s="1" t="s">
+      <c r="F32" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="42">
+      <c r="A33" t="s">
+        <v>69</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D33" t="s">
         <v>71</v>
       </c>
-      <c r="D27" t="s">
-        <v>73</v>
-      </c>
-      <c r="E27" t="s">
+      <c r="E33" t="s">
+        <v>72</v>
+      </c>
+      <c r="F33" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="42">
+      <c r="A34" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D34" t="s">
+        <v>67</v>
+      </c>
+      <c r="E34" t="s">
+        <v>45</v>
+      </c>
+      <c r="F34" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="63">
+      <c r="A35" t="s">
+        <v>64</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D35" t="s">
+        <v>63</v>
+      </c>
+      <c r="E35" t="s">
+        <v>45</v>
+      </c>
+      <c r="F35" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="126">
+      <c r="A36" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D36" t="s">
+        <v>44</v>
+      </c>
+      <c r="E36" t="s">
+        <v>109</v>
+      </c>
+      <c r="F36" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="21">
+      <c r="A37" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D37" t="s">
+        <v>17</v>
+      </c>
+      <c r="E37" t="s">
+        <v>45</v>
+      </c>
+      <c r="F37" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="21">
+      <c r="A38" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D38" t="s">
+        <v>19</v>
+      </c>
+      <c r="E38" t="s">
+        <v>45</v>
+      </c>
+      <c r="F38" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="42">
+      <c r="A39" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B39">
+        <v>2</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D39" t="s">
+        <v>23</v>
+      </c>
+      <c r="E39" t="s">
+        <v>45</v>
+      </c>
+      <c r="F39" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="21">
+      <c r="A40" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B40">
+        <v>3</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D40" t="s">
+        <v>30</v>
+      </c>
+      <c r="E40" t="s">
+        <v>45</v>
+      </c>
+      <c r="F40" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="42">
+      <c r="A41" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B41">
+        <v>4</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E41" t="s">
+        <v>45</v>
+      </c>
+      <c r="F41" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="21">
+      <c r="A42" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B42">
+        <v>5</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D42" t="s">
+        <v>22</v>
+      </c>
+      <c r="E42" t="s">
+        <v>45</v>
+      </c>
+      <c r="F42" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="21">
+      <c r="A43" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B43">
+        <v>6</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D43" t="s">
+        <v>24</v>
+      </c>
+      <c r="E43" t="s">
+        <v>45</v>
+      </c>
+      <c r="F43" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="21">
+      <c r="A44" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B44">
+        <v>7</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D44" t="s">
+        <v>26</v>
+      </c>
+      <c r="E44" t="s">
+        <v>45</v>
+      </c>
+      <c r="F44" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="126">
+      <c r="A45" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B45">
+        <v>0</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D45" t="s">
+        <v>61</v>
+      </c>
+      <c r="E45" t="s">
+        <v>45</v>
+      </c>
+      <c r="F45" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="63">
+      <c r="A46" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B46">
+        <v>0</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D46" t="s">
+        <v>5</v>
+      </c>
+      <c r="E46" t="s">
+        <v>45</v>
+      </c>
+      <c r="F46" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="42">
+      <c r="A47" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B47">
+        <v>0</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D47" t="s">
+        <v>5</v>
+      </c>
+      <c r="E47" t="s">
+        <v>45</v>
+      </c>
+      <c r="F47" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="21">
+      <c r="A48" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B48">
+        <v>0</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F27" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="42">
-      <c r="A28" t="s">
-        <v>75</v>
-      </c>
-      <c r="B28">
-        <v>0</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D28" t="s">
-        <v>77</v>
-      </c>
-      <c r="E28" t="s">
-        <v>78</v>
-      </c>
-      <c r="F28" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="105">
-      <c r="A29" t="s">
-        <v>79</v>
-      </c>
-      <c r="B29">
-        <v>0</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D29" t="s">
-        <v>73</v>
-      </c>
-      <c r="E29" t="s">
-        <v>78</v>
-      </c>
-      <c r="F29" t="s">
-        <v>74</v>
+      <c r="D48" t="s">
+        <v>5</v>
+      </c>
+      <c r="E48" t="s">
+        <v>45</v>
+      </c>
+      <c r="F48" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="84">
+      <c r="A49" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D49" t="s">
+        <v>5</v>
+      </c>
+      <c r="E49" t="s">
+        <v>45</v>
+      </c>
+      <c r="F49" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="42">
+      <c r="A50" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B50">
+        <v>0</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D50" t="s">
+        <v>60</v>
+      </c>
+      <c r="E50" t="s">
+        <v>45</v>
+      </c>
+      <c r="F50" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add imgs, signs without texts
</commit_message>
<xml_diff>
--- a/data_excel/tags.xlsx
+++ b/data_excel/tags.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jay/xidev/kanban/data_excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{32869826-2EF1-1B43-99DC-BC61E5C48369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{65083B93-1A1A-7D4F-966A-166A6837CE95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16940" yWindow="660" windowWidth="21300" windowHeight="17120" xr2:uid="{1951D371-7A8D-D346-B651-736256765602}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="407">
   <si>
     <t>img</t>
     <phoneticPr fontId="1"/>
@@ -816,109 +816,6 @@
   </si>
   <si>
     <t>IMG_4856.HEIC</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <r>
-      <t>危院！！立入禁止
-Danger!! Off-limits
-危</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Microsoft JhengHei"/>
-        <family val="2"/>
-        <charset val="128"/>
-      </rPr>
-      <t>险</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="游ゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>！！</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Microsoft JhengHei"/>
-        <family val="2"/>
-        <charset val="128"/>
-      </rPr>
-      <t>请</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="游ゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>别</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Microsoft JhengHei"/>
-        <family val="2"/>
-        <charset val="128"/>
-      </rPr>
-      <t>进</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="游ゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">入
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Malgun Gothic"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>위험하다</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="游ゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">!! </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Malgun Gothic"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>출입금지</t>
-    </r>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -5768,6 +5665,529 @@
   </si>
   <si>
     <t>IMG_1663.HEIC</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>危険！！立入禁止
+Danger!! Off-limits
+危</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Microsoft JhengHei"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t>险</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>！！</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Microsoft JhengHei"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t>请</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>别</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Microsoft JhengHei"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t>进</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">入
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>위험하다</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">!! </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>출입금지</t>
+    </r>
+    <rPh sb="0" eb="2">
+      <t xml:space="preserve">キケン </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>大和西大寺</t>
+    <rPh sb="0" eb="2">
+      <t xml:space="preserve">ヤマト </t>
+    </rPh>
+    <rPh sb="2" eb="5">
+      <t xml:space="preserve">サイダイジ </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>IMG_1525.HEIC</t>
+  </si>
+  <si>
+    <t>IMG_1405.HEIC</t>
+  </si>
+  <si>
+    <t>IMG_1395.HEIC</t>
+  </si>
+  <si>
+    <t>IMG_1217.heic</t>
+  </si>
+  <si>
+    <t>IMG_1208.HEIC</t>
+  </si>
+  <si>
+    <t>IMG_1179.heic</t>
+  </si>
+  <si>
+    <t>IMG_1177.HEIC</t>
+  </si>
+  <si>
+    <t>IMG_1176.HEIC</t>
+  </si>
+  <si>
+    <t>自転車・バイク
+駐輪禁止</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>赤丸斜線|自転車|バイク</t>
+    <rPh sb="0" eb="4">
+      <t>🔴</t>
+    </rPh>
+    <rPh sb="5" eb="8">
+      <t xml:space="preserve">ジテンシャ </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">線路内立ち入り禁止
+Do not enter the tracks
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Microsoft JhengHei"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t>严</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>禁</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Microsoft JhengHei"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t>进</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>入</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Microsoft JhengHei"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t>铁</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">路内
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>선로</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>내</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>출입금지</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+線路へ物を落とされたときは係員にお知らせください
+If you drop something on the tracks, please contact station staff.</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>赤丸斜線|電車|線路|走る人</t>
+    <rPh sb="0" eb="1">
+      <t xml:space="preserve">アカマル </t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t xml:space="preserve">デンシャ </t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t xml:space="preserve">センロ </t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t xml:space="preserve">ハシルヒト </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>新大宮</t>
+    <rPh sb="0" eb="3">
+      <t xml:space="preserve">シンオオミヤ </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>飲み水ではありません。
+Do not drink.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>赤丸斜線|蛇口|コップに水</t>
+    <rPh sb="0" eb="1">
+      <t>🔴</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t xml:space="preserve">ジャグチ </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>新幹線のぞみ</t>
+    <rPh sb="0" eb="1">
+      <t xml:space="preserve">シンカンセン </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>NO FOOD NO DRINK
+飲食はご遠慮ください</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>赤丸斜線|カップ飲料|串</t>
+    <rPh sb="0" eb="4">
+      <t>アカマ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t xml:space="preserve">インリョウ </t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>🪮</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>https://x.com/xiPJ/status/2004831692180410394</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>赤丸斜線|自転車</t>
+    <rPh sb="0" eb="4">
+      <t>🔴</t>
+    </rPh>
+    <rPh sb="5" eb="8">
+      <t xml:space="preserve">ジテンシャ </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>自転車通行は 終日通行禁止
+《三条寺町～河原町）
+中京警察署
+三条商店街(振)
+駐輪・駐車禁止</t>
+    <rPh sb="8" eb="9">
+      <t xml:space="preserve">ニチ </t>
+    </rPh>
+    <rPh sb="40" eb="42">
+      <t xml:space="preserve">チュウリン </t>
+    </rPh>
+    <rPh sb="43" eb="45">
+      <t xml:space="preserve">チュウシャ </t>
+    </rPh>
+    <rPh sb="45" eb="47">
+      <t xml:space="preserve">キンシ </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ここはゴミ箱ではありません
+ごみを捨てないでください
+Don't throw trash here</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>自立|看板</t>
+    <rPh sb="0" eb="1">
+      <t xml:space="preserve">ジリツカンバン </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>赤丸斜線|手|丸めた紙</t>
+    <rPh sb="0" eb="4">
+      <t>🔴</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>☚</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t xml:space="preserve">マルメタカミ </t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>🪮</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>矢印|エスカレーターに乗る人|上矢印</t>
+    <rPh sb="0" eb="2">
+      <t xml:space="preserve">ヤジルシ </t>
+    </rPh>
+    <rPh sb="15" eb="18">
+      <t xml:space="preserve">ウエヤジルシ </t>
+    </rPh>
+    <rPh sb="28" eb="29">
+      <t xml:space="preserve">ヒトビト </t>
+    </rPh>
+    <rPh sb="31" eb="35">
+      <t xml:space="preserve">ジョウゲヤジルシ </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>矢印|エレベーターに乗る人々|上下矢印</t>
+    <rPh sb="0" eb="2">
+      <t xml:space="preserve">ヤジルシ </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>赤丸斜線|タバコ</t>
+    <rPh sb="0" eb="4">
+      <t>🔴</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>斜線|タバコ</t>
+    <rPh sb="0" eb="2">
+      <t xml:space="preserve">シャセン </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>斜線|犬</t>
+    <rPh sb="0" eb="1">
+      <t xml:space="preserve">シャセン </t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t xml:space="preserve">イヌ </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>斜線|カップ飲料|ハンバーガー</t>
+    <rPh sb="0" eb="2">
+      <t xml:space="preserve">シャセン </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>斜線|カメラ</t>
+    <rPh sb="0" eb="2">
+      <t xml:space="preserve">シャセン </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>当店ではお車でご来店のお客様への酒類の販売をお断りしております。</t>
+    <rPh sb="0" eb="1">
+      <t xml:space="preserve">トウテンデハ </t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t xml:space="preserve">サケルイ </t>
+    </rPh>
+    <rPh sb="19" eb="21">
+      <t xml:space="preserve">ハンバイヲ </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>赤丸斜線|徳利とお猪口|車</t>
+    <rPh sb="0" eb="4">
+      <t>🔴</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t xml:space="preserve">トックリトオチョコ </t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t xml:space="preserve">クルマ </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>柱|看板</t>
+    <rPh sb="0" eb="1">
+      <t xml:space="preserve">ハシラ </t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t xml:space="preserve">カンバン </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>IMG_1161.jpg</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -6276,10 +6696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0244D4E8-F443-D54E-A975-960F8853E327}">
-  <dimension ref="A1:H127"/>
+  <dimension ref="A1:H144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="106" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="106" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -6312,70 +6732,70 @@
         <v>41</v>
       </c>
       <c r="G1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="273">
       <c r="A2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" t="s">
         <v>332</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>333</v>
       </c>
-      <c r="F2" t="s">
-        <v>334</v>
-      </c>
       <c r="G2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="84">
       <c r="A3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" t="s">
         <v>336</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>337</v>
       </c>
-      <c r="F3" t="s">
-        <v>338</v>
-      </c>
       <c r="G3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="126">
       <c r="A4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>339</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>340</v>
       </c>
       <c r="E4" t="s">
         <v>70</v>
@@ -6384,133 +6804,133 @@
         <v>46</v>
       </c>
       <c r="G4" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="147">
       <c r="A5" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E5" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F5" t="s">
         <v>40</v>
       </c>
       <c r="G5" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="147">
       <c r="A6" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" t="s">
         <v>345</v>
-      </c>
-      <c r="E6" t="s">
-        <v>346</v>
       </c>
       <c r="F6" t="s">
         <v>40</v>
       </c>
       <c r="G6" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="147">
       <c r="A7" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F7" t="s">
         <v>39</v>
       </c>
       <c r="G7" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="147">
       <c r="A8" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B8">
         <v>0</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>351</v>
-      </c>
       <c r="E8" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F8" t="s">
         <v>40</v>
       </c>
       <c r="G8" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="147">
       <c r="A9" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B9">
         <v>0</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="E9" t="s">
+        <v>345</v>
+      </c>
+      <c r="F9" t="s">
+        <v>352</v>
+      </c>
+      <c r="G9" t="s">
         <v>354</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="E9" t="s">
-        <v>346</v>
-      </c>
-      <c r="F9" t="s">
-        <v>353</v>
-      </c>
-      <c r="G9" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="147">
       <c r="A10" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B10">
         <v>0</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>5</v>
@@ -6522,41 +6942,41 @@
         <v>36</v>
       </c>
       <c r="G10" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="63">
       <c r="A11" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B11">
         <v>0</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>364</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>365</v>
       </c>
       <c r="E11" t="s">
         <v>45</v>
       </c>
       <c r="F11" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G11" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="21">
       <c r="A12" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B12">
         <v>0</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>5</v>
@@ -6565,984 +6985,959 @@
         <v>45</v>
       </c>
       <c r="F12" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G12" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="147">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="42">
       <c r="A13" t="s">
-        <v>179</v>
+        <v>371</v>
       </c>
       <c r="B13">
         <v>0</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>202</v>
+        <v>379</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>203</v>
+        <v>380</v>
       </c>
       <c r="E13" t="s">
-        <v>201</v>
+        <v>45</v>
       </c>
       <c r="F13" t="s">
-        <v>212</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="168">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="126">
       <c r="A14" t="s">
-        <v>285</v>
+        <v>372</v>
       </c>
       <c r="B14">
         <v>0</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>286</v>
+        <v>381</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>5</v>
+        <v>382</v>
       </c>
       <c r="E14" t="s">
-        <v>294</v>
+        <v>45</v>
       </c>
       <c r="F14" t="s">
-        <v>281</v>
-      </c>
-      <c r="H14" s="4"/>
+        <v>36</v>
+      </c>
+      <c r="G14" t="s">
+        <v>383</v>
+      </c>
     </row>
     <row r="15" spans="1:8" ht="42">
       <c r="A15" t="s">
-        <v>282</v>
+        <v>373</v>
       </c>
       <c r="B15">
         <v>0</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>349</v>
+        <v>384</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>283</v>
+        <v>385</v>
       </c>
       <c r="E15" t="s">
-        <v>284</v>
+        <v>70</v>
       </c>
       <c r="F15" t="s">
-        <v>66</v>
-      </c>
-      <c r="H15" s="4"/>
-    </row>
-    <row r="16" spans="1:8" ht="63">
+        <v>36</v>
+      </c>
+      <c r="G15" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="42">
       <c r="A16" t="s">
-        <v>277</v>
+        <v>374</v>
       </c>
       <c r="B16">
         <v>0</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>278</v>
+        <v>387</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>279</v>
+        <v>388</v>
       </c>
       <c r="E16" t="s">
-        <v>280</v>
+        <v>200</v>
       </c>
       <c r="F16" t="s">
-        <v>281</v>
-      </c>
-      <c r="H16" s="4"/>
-    </row>
-    <row r="17" spans="1:8" ht="168">
+        <v>39</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="105">
       <c r="A17" t="s">
-        <v>179</v>
+        <v>375</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>204</v>
+        <v>391</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>5</v>
+        <v>390</v>
       </c>
       <c r="E17" t="s">
-        <v>302</v>
+        <v>45</v>
       </c>
       <c r="F17" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="63">
       <c r="A18" t="s">
-        <v>287</v>
+        <v>376</v>
       </c>
       <c r="B18">
         <v>0</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>288</v>
+        <v>392</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>290</v>
+        <v>5</v>
       </c>
       <c r="E18" t="s">
-        <v>293</v>
+        <v>70</v>
       </c>
       <c r="F18" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="42">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="21">
       <c r="A19" t="s">
-        <v>287</v>
+        <v>377</v>
       </c>
       <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="E19" t="s">
+        <v>393</v>
+      </c>
+      <c r="F19" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="21">
+      <c r="A20" t="s">
+        <v>377</v>
+      </c>
+      <c r="B20">
         <v>1</v>
       </c>
-      <c r="C19" s="7" t="s">
-        <v>289</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="E19" t="s">
-        <v>293</v>
-      </c>
-      <c r="F19" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="63">
-      <c r="A20" t="s">
-        <v>180</v>
-      </c>
-      <c r="B20">
-        <v>0</v>
-      </c>
       <c r="C20" s="1" t="s">
-        <v>207</v>
+        <v>393</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>5</v>
+        <v>397</v>
       </c>
       <c r="E20" t="s">
-        <v>303</v>
+        <v>393</v>
       </c>
       <c r="F20" t="s">
-        <v>208</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="42">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="21">
       <c r="A21" t="s">
-        <v>181</v>
+        <v>377</v>
       </c>
       <c r="B21">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>210</v>
+        <v>393</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>211</v>
+        <v>395</v>
       </c>
       <c r="E21" t="s">
-        <v>304</v>
+        <v>393</v>
       </c>
       <c r="F21" t="s">
-        <v>49</v>
-      </c>
-      <c r="H21" s="4" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="42">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="21">
       <c r="A22" t="s">
-        <v>181</v>
+        <v>377</v>
       </c>
       <c r="B22">
-        <v>1</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>213</v>
+        <v>3</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>393</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>214</v>
+        <v>398</v>
       </c>
       <c r="E22" t="s">
-        <v>304</v>
+        <v>393</v>
       </c>
       <c r="F22" t="s">
-        <v>49</v>
-      </c>
-      <c r="H22" s="4"/>
-    </row>
-    <row r="23" spans="1:8" ht="42">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="21">
       <c r="A23" t="s">
-        <v>181</v>
+        <v>377</v>
       </c>
       <c r="B23">
-        <v>2</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>215</v>
+        <v>4</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>393</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>216</v>
+        <v>390</v>
       </c>
       <c r="E23" t="s">
-        <v>45</v>
+        <v>393</v>
       </c>
       <c r="F23" t="s">
-        <v>49</v>
-      </c>
-      <c r="H23" s="4"/>
-    </row>
-    <row r="24" spans="1:8" ht="42">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="21">
       <c r="A24" t="s">
-        <v>182</v>
+        <v>378</v>
       </c>
       <c r="B24">
         <v>0</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>217</v>
+        <v>393</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>5</v>
+        <v>399</v>
       </c>
       <c r="E24" t="s">
-        <v>70</v>
+        <v>393</v>
       </c>
       <c r="F24" t="s">
-        <v>234</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="84">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="21">
       <c r="A25" t="s">
-        <v>182</v>
+        <v>378</v>
       </c>
       <c r="B25">
         <v>1</v>
       </c>
-      <c r="C25" s="7" t="s">
-        <v>218</v>
+      <c r="C25" s="1" t="s">
+        <v>393</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>219</v>
+        <v>400</v>
       </c>
       <c r="E25" t="s">
-        <v>305</v>
+        <v>393</v>
       </c>
       <c r="F25" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="84">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="21">
       <c r="A26" t="s">
-        <v>183</v>
+        <v>378</v>
       </c>
       <c r="B26">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>220</v>
+        <v>393</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>221</v>
+        <v>401</v>
       </c>
       <c r="E26" t="s">
-        <v>314</v>
+        <v>393</v>
       </c>
       <c r="F26" t="s">
-        <v>49</v>
-      </c>
-      <c r="H26" s="4" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="105">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="21">
       <c r="A27" t="s">
-        <v>184</v>
+        <v>378</v>
       </c>
       <c r="B27">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>222</v>
+        <v>393</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>223</v>
+        <v>402</v>
       </c>
       <c r="E27" t="s">
-        <v>306</v>
+        <v>393</v>
       </c>
       <c r="F27" t="s">
-        <v>39</v>
-      </c>
-      <c r="H27" s="4" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="82">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="21">
       <c r="A28" t="s">
-        <v>185</v>
+        <v>406</v>
       </c>
       <c r="B28">
         <v>0</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>227</v>
+        <v>393</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>5</v>
+        <v>398</v>
       </c>
       <c r="E28" t="s">
-        <v>310</v>
+        <v>393</v>
       </c>
       <c r="F28" t="s">
-        <v>49</v>
-      </c>
-      <c r="H28" s="4" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="105">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="21">
       <c r="A29" t="s">
-        <v>186</v>
+        <v>406</v>
       </c>
       <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="E29" t="s">
+        <v>45</v>
+      </c>
+      <c r="F29" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="147">
+      <c r="A30" t="s">
+        <v>178</v>
+      </c>
+      <c r="B30">
         <v>0</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E29" t="s">
-        <v>292</v>
-      </c>
-      <c r="F29" t="s">
-        <v>39</v>
-      </c>
-      <c r="H29" s="4" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="42">
-      <c r="A30" t="s">
-        <v>186</v>
-      </c>
-      <c r="B30">
-        <v>1</v>
-      </c>
       <c r="C30" s="1" t="s">
-        <v>229</v>
+        <v>201</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>19</v>
+        <v>202</v>
       </c>
       <c r="E30" t="s">
-        <v>316</v>
+        <v>200</v>
       </c>
       <c r="F30" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="21">
+        <v>211</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="168">
       <c r="A31" t="s">
-        <v>187</v>
+        <v>284</v>
       </c>
       <c r="B31">
         <v>0</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>230</v>
+        <v>285</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>231</v>
+        <v>5</v>
       </c>
       <c r="E31" t="s">
-        <v>232</v>
+        <v>293</v>
       </c>
       <c r="F31" t="s">
-        <v>233</v>
-      </c>
-      <c r="H31" s="4" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="147">
+        <v>280</v>
+      </c>
+      <c r="H31" s="4"/>
+    </row>
+    <row r="32" spans="1:8" ht="42">
       <c r="A32" t="s">
-        <v>188</v>
+        <v>281</v>
       </c>
       <c r="B32">
         <v>0</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>235</v>
+        <v>348</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>236</v>
+        <v>282</v>
       </c>
       <c r="E32" t="s">
-        <v>307</v>
+        <v>283</v>
       </c>
       <c r="F32" t="s">
-        <v>39</v>
-      </c>
-      <c r="H32" s="4" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="124">
+        <v>66</v>
+      </c>
+      <c r="H32" s="4"/>
+    </row>
+    <row r="33" spans="1:8" ht="63">
       <c r="A33" t="s">
-        <v>189</v>
+        <v>276</v>
       </c>
       <c r="B33">
         <v>0</v>
       </c>
-      <c r="C33" s="8" t="s">
-        <v>237</v>
+      <c r="C33" s="1" t="s">
+        <v>277</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>240</v>
+        <v>278</v>
       </c>
       <c r="E33" t="s">
-        <v>239</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="H33" s="4" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="84">
+        <v>279</v>
+      </c>
+      <c r="F33" t="s">
+        <v>280</v>
+      </c>
+      <c r="H33" s="4"/>
+    </row>
+    <row r="34" spans="1:8" ht="168">
       <c r="A34" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E34" t="s">
+        <v>301</v>
+      </c>
+      <c r="F34" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="63">
+      <c r="A35" t="s">
+        <v>286</v>
+      </c>
+      <c r="B35">
         <v>0</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="E34" t="s">
-        <v>308</v>
-      </c>
-      <c r="F34" t="s">
-        <v>40</v>
-      </c>
-      <c r="H34" s="4" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="84">
-      <c r="A35" t="s">
-        <v>190</v>
-      </c>
-      <c r="B35">
+      <c r="C35" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="E35" t="s">
+        <v>292</v>
+      </c>
+      <c r="F35" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="42">
+      <c r="A36" t="s">
+        <v>286</v>
+      </c>
+      <c r="B36">
         <v>1</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="E35" t="s">
-        <v>308</v>
-      </c>
-      <c r="F35" t="s">
-        <v>40</v>
-      </c>
-      <c r="H35" s="4"/>
-    </row>
-    <row r="36" spans="1:8" ht="84">
-      <c r="A36" t="s">
-        <v>190</v>
-      </c>
-      <c r="B36">
+      <c r="C36" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="E36" t="s">
+        <v>292</v>
+      </c>
+      <c r="F36" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="63">
+      <c r="A37" t="s">
+        <v>179</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E37" t="s">
+        <v>302</v>
+      </c>
+      <c r="F37" t="s">
+        <v>207</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="42">
+      <c r="A38" t="s">
+        <v>180</v>
+      </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="E38" t="s">
+        <v>303</v>
+      </c>
+      <c r="F38" t="s">
+        <v>49</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="42">
+      <c r="A39" t="s">
+        <v>180</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="E39" t="s">
+        <v>303</v>
+      </c>
+      <c r="F39" t="s">
+        <v>49</v>
+      </c>
+      <c r="H39" s="4"/>
+    </row>
+    <row r="40" spans="1:8" ht="42">
+      <c r="A40" t="s">
+        <v>180</v>
+      </c>
+      <c r="B40">
         <v>2</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="E36" t="s">
-        <v>308</v>
-      </c>
-      <c r="F36" t="s">
-        <v>40</v>
-      </c>
-      <c r="H36" s="4"/>
-    </row>
-    <row r="37" spans="1:8" ht="84">
-      <c r="A37" t="s">
-        <v>190</v>
-      </c>
-      <c r="B37">
-        <v>3</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="E37" t="s">
-        <v>308</v>
-      </c>
-      <c r="F37" t="s">
-        <v>40</v>
-      </c>
-      <c r="H37" s="4"/>
-    </row>
-    <row r="38" spans="1:8" ht="63">
-      <c r="A38" t="s">
-        <v>190</v>
-      </c>
-      <c r="B38">
-        <v>4</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="E38" t="s">
-        <v>309</v>
-      </c>
-      <c r="F38" t="s">
-        <v>40</v>
-      </c>
-      <c r="H38" s="4"/>
-    </row>
-    <row r="39" spans="1:8" ht="84">
-      <c r="A39" t="s">
-        <v>190</v>
-      </c>
-      <c r="B39">
-        <v>5</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="E39" t="s">
-        <v>308</v>
-      </c>
-      <c r="F39" t="s">
-        <v>40</v>
-      </c>
-      <c r="H39" s="4"/>
-    </row>
-    <row r="40" spans="1:8" ht="21">
-      <c r="A40" t="s">
-        <v>190</v>
-      </c>
-      <c r="B40">
-        <v>6</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>253</v>
+      <c r="C40" s="7" t="s">
+        <v>214</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>5</v>
+        <v>215</v>
       </c>
       <c r="E40" t="s">
         <v>45</v>
       </c>
       <c r="F40" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="H40" s="4"/>
     </row>
-    <row r="41" spans="1:8" ht="105">
+    <row r="41" spans="1:8" ht="42">
       <c r="A41" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B41">
         <v>0</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>275</v>
+        <v>216</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E41" t="s">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="F41" t="s">
-        <v>49</v>
+        <v>233</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="21">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="84">
       <c r="A42" t="s">
-        <v>272</v>
+        <v>181</v>
       </c>
       <c r="B42">
-        <v>0</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>273</v>
+        <v>1</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>217</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>5</v>
+        <v>218</v>
       </c>
       <c r="E42" t="s">
-        <v>45</v>
+        <v>304</v>
       </c>
       <c r="F42" t="s">
-        <v>36</v>
-      </c>
-      <c r="H42" s="4" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" ht="82">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="84">
       <c r="A43" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="B43">
         <v>0</v>
       </c>
-      <c r="C43" s="3" t="s">
-        <v>254</v>
+      <c r="C43" s="1" t="s">
+        <v>219</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>255</v>
+        <v>220</v>
       </c>
       <c r="E43" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="F43" t="s">
-        <v>300</v>
+        <v>49</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="42">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="105">
       <c r="A44" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="B44">
         <v>0</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>268</v>
+        <v>221</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>5</v>
+        <v>222</v>
       </c>
       <c r="E44" t="s">
-        <v>45</v>
+        <v>305</v>
       </c>
       <c r="F44" t="s">
         <v>39</v>
       </c>
-      <c r="G44" t="s">
-        <v>269</v>
-      </c>
       <c r="H44" s="4" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" ht="105">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="82">
       <c r="A45" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="B45">
         <v>0</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>264</v>
+        <v>226</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>263</v>
+        <v>5</v>
       </c>
       <c r="E45" t="s">
-        <v>45</v>
+        <v>309</v>
       </c>
       <c r="F45" t="s">
-        <v>301</v>
+        <v>49</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" ht="42">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="105">
       <c r="A46" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="B46">
         <v>0</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>262</v>
+        <v>227</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E46" t="s">
-        <v>45</v>
+        <v>291</v>
       </c>
       <c r="F46" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>261</v>
+        <v>161</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="42">
       <c r="A47" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="B47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>260</v>
+        <v>228</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="E47" t="s">
-        <v>45</v>
+        <v>315</v>
       </c>
       <c r="F47" t="s">
-        <v>49</v>
-      </c>
-      <c r="H47" s="4" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" ht="42">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="21">
       <c r="A48" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="B48">
         <v>0</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>265</v>
+        <v>229</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>266</v>
+        <v>230</v>
       </c>
       <c r="E48" t="s">
-        <v>45</v>
+        <v>231</v>
       </c>
       <c r="F48" t="s">
-        <v>49</v>
+        <v>232</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" ht="63">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="147">
       <c r="A49" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="B49">
         <v>0</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>256</v>
+        <v>234</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>5</v>
+        <v>235</v>
       </c>
       <c r="E49" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="F49" t="s">
-        <v>257</v>
+        <v>39</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" ht="63">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="124">
       <c r="A50" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="B50">
         <v>0</v>
       </c>
-      <c r="C50" s="1" t="s">
-        <v>200</v>
+      <c r="C50" s="8" t="s">
+        <v>236</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>5</v>
+        <v>239</v>
       </c>
       <c r="E50" t="s">
-        <v>70</v>
-      </c>
-      <c r="F50" t="s">
-        <v>49</v>
+        <v>238</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>237</v>
       </c>
       <c r="H50" s="4" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" ht="42">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="84">
       <c r="A51" t="s">
-        <v>121</v>
+        <v>189</v>
       </c>
       <c r="B51">
         <v>0</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>130</v>
+        <v>240</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>5</v>
+        <v>241</v>
       </c>
       <c r="E51" t="s">
-        <v>45</v>
+        <v>307</v>
       </c>
       <c r="F51" t="s">
-        <v>36</v>
+        <v>40</v>
+      </c>
+      <c r="H51" s="4" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="84">
       <c r="A52" t="s">
-        <v>122</v>
+        <v>189</v>
       </c>
       <c r="B52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>131</v>
+        <v>242</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>5</v>
+        <v>243</v>
       </c>
       <c r="E52" t="s">
-        <v>45</v>
+        <v>307</v>
       </c>
       <c r="F52" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" ht="168">
+        <v>40</v>
+      </c>
+      <c r="H52" s="4"/>
+    </row>
+    <row r="53" spans="1:8" ht="84">
       <c r="A53" t="s">
-        <v>123</v>
+        <v>189</v>
       </c>
       <c r="B53">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>135</v>
+        <v>244</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>5</v>
+        <v>245</v>
       </c>
       <c r="E53" t="s">
-        <v>45</v>
+        <v>307</v>
       </c>
       <c r="F53" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" ht="42">
+        <v>40</v>
+      </c>
+      <c r="H53" s="4"/>
+    </row>
+    <row r="54" spans="1:8" ht="84">
       <c r="A54" t="s">
-        <v>123</v>
+        <v>189</v>
       </c>
       <c r="B54">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>136</v>
+        <v>246</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>5</v>
+        <v>249</v>
       </c>
       <c r="E54" t="s">
-        <v>45</v>
+        <v>307</v>
       </c>
       <c r="F54" t="s">
-        <v>39</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="H54" s="4"/>
     </row>
     <row r="55" spans="1:8" ht="63">
       <c r="A55" t="s">
-        <v>123</v>
+        <v>189</v>
       </c>
       <c r="B55">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>137</v>
+        <v>247</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>5</v>
+        <v>250</v>
       </c>
       <c r="E55" t="s">
-        <v>45</v>
+        <v>308</v>
       </c>
       <c r="F55" t="s">
-        <v>39</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="H55" s="4"/>
     </row>
     <row r="56" spans="1:8" ht="84">
       <c r="A56" t="s">
-        <v>123</v>
+        <v>189</v>
       </c>
       <c r="B56">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>133</v>
+        <v>248</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>134</v>
+        <v>251</v>
       </c>
       <c r="E56" t="s">
-        <v>45</v>
+        <v>307</v>
       </c>
       <c r="F56" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" ht="84">
+        <v>40</v>
+      </c>
+      <c r="H56" s="4"/>
+    </row>
+    <row r="57" spans="1:8" ht="21">
       <c r="A57" t="s">
-        <v>124</v>
+        <v>189</v>
       </c>
       <c r="B57">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>139</v>
+        <v>252</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>141</v>
+        <v>5</v>
       </c>
       <c r="E57" t="s">
         <v>45</v>
@@ -7550,36 +7945,40 @@
       <c r="F57" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" ht="42">
+      <c r="H57" s="4"/>
+    </row>
+    <row r="58" spans="1:8" ht="105">
       <c r="A58" t="s">
-        <v>124</v>
+        <v>190</v>
       </c>
       <c r="B58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>138</v>
+        <v>274</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>142</v>
+        <v>5</v>
       </c>
       <c r="E58" t="s">
         <v>45</v>
       </c>
       <c r="F58" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" ht="84">
+        <v>49</v>
+      </c>
+      <c r="H58" s="4" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="21">
       <c r="A59" t="s">
-        <v>125</v>
+        <v>271</v>
       </c>
       <c r="B59">
         <v>0</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>143</v>
+        <v>272</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>5</v>
@@ -7588,38 +7987,44 @@
         <v>45</v>
       </c>
       <c r="F59" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" ht="168">
+        <v>36</v>
+      </c>
+      <c r="H59" s="4" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="82">
       <c r="A60" t="s">
-        <v>126</v>
+        <v>191</v>
       </c>
       <c r="B60">
         <v>0</v>
       </c>
-      <c r="C60" s="1" t="s">
-        <v>144</v>
+      <c r="C60" s="3" t="s">
+        <v>253</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>145</v>
+        <v>254</v>
       </c>
       <c r="E60" t="s">
-        <v>45</v>
+        <v>311</v>
       </c>
       <c r="F60" t="s">
-        <v>147</v>
+        <v>299</v>
+      </c>
+      <c r="H60" s="4" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="42">
       <c r="A61" t="s">
-        <v>127</v>
+        <v>192</v>
       </c>
       <c r="B61">
         <v>0</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>149</v>
+        <v>267</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>5</v>
@@ -7628,38 +8033,47 @@
         <v>45</v>
       </c>
       <c r="F61" t="s">
-        <v>148</v>
+        <v>39</v>
+      </c>
+      <c r="G61" t="s">
+        <v>268</v>
+      </c>
+      <c r="H61" s="4" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="105">
       <c r="A62" t="s">
-        <v>128</v>
+        <v>193</v>
       </c>
       <c r="B62">
         <v>0</v>
       </c>
-      <c r="C62" s="3" t="s">
-        <v>150</v>
+      <c r="C62" s="1" t="s">
+        <v>263</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>5</v>
+        <v>262</v>
       </c>
       <c r="E62" t="s">
         <v>45</v>
       </c>
       <c r="F62" t="s">
-        <v>36</v>
+        <v>300</v>
+      </c>
+      <c r="H62" s="4" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="42">
       <c r="A63" t="s">
-        <v>128</v>
+        <v>194</v>
       </c>
       <c r="B63">
-        <v>1</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>151</v>
+        <v>0</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>261</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>5</v>
@@ -7668,18 +8082,21 @@
         <v>45</v>
       </c>
       <c r="F63" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" ht="63">
+        <v>40</v>
+      </c>
+      <c r="H63" s="4" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="42">
       <c r="A64" t="s">
-        <v>129</v>
+        <v>195</v>
       </c>
       <c r="B64">
         <v>0</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>152</v>
+        <v>259</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>5</v>
@@ -7688,58 +8105,67 @@
         <v>45</v>
       </c>
       <c r="F64" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" ht="21">
+        <v>49</v>
+      </c>
+      <c r="H64" s="4" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="42">
       <c r="A65" t="s">
-        <v>78</v>
+        <v>196</v>
       </c>
       <c r="B65">
         <v>0</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>79</v>
+        <v>264</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>5</v>
+        <v>265</v>
       </c>
       <c r="E65" t="s">
         <v>45</v>
       </c>
       <c r="F65" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" ht="84">
+        <v>49</v>
+      </c>
+      <c r="H65" s="4" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="63">
       <c r="A66" t="s">
-        <v>78</v>
+        <v>197</v>
       </c>
       <c r="B66">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>80</v>
+        <v>255</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>81</v>
+        <v>5</v>
       </c>
       <c r="E66" t="s">
-        <v>70</v>
+        <v>314</v>
       </c>
       <c r="F66" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" ht="21">
+        <v>256</v>
+      </c>
+      <c r="H66" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="63">
       <c r="A67" t="s">
-        <v>78</v>
+        <v>198</v>
       </c>
       <c r="B67">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>82</v>
+        <v>199</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>5</v>
@@ -7748,218 +8174,221 @@
         <v>70</v>
       </c>
       <c r="F67" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" ht="42">
+        <v>49</v>
+      </c>
+      <c r="H67" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="42">
       <c r="A68" t="s">
-        <v>78</v>
+        <v>120</v>
       </c>
       <c r="B68">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>83</v>
+        <v>129</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>92</v>
+        <v>5</v>
       </c>
       <c r="E68" t="s">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="F68" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="42">
+    <row r="69" spans="1:8" ht="84">
       <c r="A69" t="s">
-        <v>78</v>
+        <v>121</v>
       </c>
       <c r="B69">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>84</v>
+        <v>130</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>93</v>
+        <v>5</v>
       </c>
       <c r="E69" t="s">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="F69" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" ht="42">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="168">
       <c r="A70" t="s">
-        <v>78</v>
+        <v>122</v>
       </c>
       <c r="B70">
+        <v>0</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D70" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C70" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>94</v>
-      </c>
       <c r="E70" t="s">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="F70" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" ht="42">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="42">
       <c r="A71" t="s">
-        <v>78</v>
+        <v>122</v>
       </c>
       <c r="B71">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>86</v>
+        <v>135</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="E71" t="s">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="F71" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" ht="42">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" ht="63">
       <c r="A72" t="s">
-        <v>78</v>
+        <v>122</v>
       </c>
       <c r="B72">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>87</v>
+        <v>136</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>95</v>
+        <v>5</v>
       </c>
       <c r="E72" t="s">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="F72" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" ht="42">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="84">
       <c r="A73" t="s">
-        <v>78</v>
+        <v>122</v>
       </c>
       <c r="B73">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>88</v>
+        <v>132</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>96</v>
+        <v>133</v>
       </c>
       <c r="E73" t="s">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="F73" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" ht="42">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="84">
       <c r="A74" t="s">
-        <v>78</v>
+        <v>123</v>
       </c>
       <c r="B74">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>89</v>
+        <v>138</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>97</v>
+        <v>140</v>
       </c>
       <c r="E74" t="s">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="F74" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" ht="168">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="42">
       <c r="A75" t="s">
-        <v>78</v>
+        <v>123</v>
       </c>
       <c r="B75">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>90</v>
+        <v>137</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>5</v>
+        <v>141</v>
       </c>
       <c r="E75" t="s">
         <v>45</v>
       </c>
       <c r="F75" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" ht="42">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="84">
       <c r="A76" t="s">
-        <v>78</v>
+        <v>124</v>
       </c>
       <c r="B76">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>91</v>
+        <v>142</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E76" t="s">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="F76" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" ht="42">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" ht="168">
       <c r="A77" t="s">
-        <v>99</v>
+        <v>125</v>
       </c>
       <c r="B77">
         <v>0</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>98</v>
+        <v>143</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>105</v>
+        <v>144</v>
       </c>
       <c r="E77" t="s">
         <v>45</v>
       </c>
       <c r="F77" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" ht="42">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" ht="42">
       <c r="A78" t="s">
-        <v>100</v>
+        <v>126</v>
       </c>
       <c r="B78">
         <v>0</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>101</v>
+        <v>148</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>5</v>
@@ -7968,38 +8397,38 @@
         <v>45</v>
       </c>
       <c r="F78" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" ht="84">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="105">
       <c r="A79" t="s">
-        <v>103</v>
+        <v>127</v>
       </c>
       <c r="B79">
         <v>0</v>
       </c>
-      <c r="C79" s="1" t="s">
-        <v>104</v>
+      <c r="C79" s="3" t="s">
+        <v>149</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>106</v>
+        <v>5</v>
       </c>
       <c r="E79" t="s">
-        <v>310</v>
+        <v>45</v>
       </c>
       <c r="F79" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" ht="63">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="42">
       <c r="A80" t="s">
-        <v>107</v>
+        <v>127</v>
       </c>
       <c r="B80">
-        <v>0</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>108</v>
+        <v>1</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>150</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>5</v>
@@ -8008,38 +8437,38 @@
         <v>45</v>
       </c>
       <c r="F80" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" ht="126">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="63">
       <c r="A81" t="s">
-        <v>109</v>
+        <v>128</v>
       </c>
       <c r="B81">
         <v>0</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>110</v>
+        <v>151</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>111</v>
+        <v>5</v>
       </c>
       <c r="E81" t="s">
         <v>45</v>
       </c>
       <c r="F81" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" ht="42">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" ht="21">
       <c r="A82" t="s">
-        <v>109</v>
+        <v>78</v>
       </c>
       <c r="B82">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>112</v>
+        <v>79</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>5</v>
@@ -8048,198 +8477,201 @@
         <v>45</v>
       </c>
       <c r="F82" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" ht="147">
+        <v>36</v>
+      </c>
+      <c r="G82" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="84">
       <c r="A83" t="s">
-        <v>113</v>
+        <v>78</v>
       </c>
       <c r="B83">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>115</v>
+        <v>81</v>
       </c>
       <c r="E83" t="s">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="F83" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" ht="105">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="21">
       <c r="A84" t="s">
-        <v>116</v>
+        <v>78</v>
       </c>
       <c r="B84">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>117</v>
+        <v>82</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E84" t="s">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="F84" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" ht="42">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="42">
       <c r="A85" t="s">
-        <v>296</v>
+        <v>78</v>
       </c>
       <c r="B85">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>295</v>
+        <v>83</v>
       </c>
       <c r="D85" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E85" t="s">
+        <v>70</v>
+      </c>
+      <c r="F85" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" ht="42">
+      <c r="A86" t="s">
+        <v>78</v>
+      </c>
+      <c r="B86">
+        <v>4</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E86" t="s">
+        <v>70</v>
+      </c>
+      <c r="F86" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" ht="42">
+      <c r="A87" t="s">
+        <v>78</v>
+      </c>
+      <c r="B87">
         <v>5</v>
       </c>
-      <c r="E85" t="s">
-        <v>297</v>
-      </c>
-      <c r="F85" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" ht="42">
-      <c r="A86" t="s">
-        <v>317</v>
-      </c>
-      <c r="B86">
-        <v>0</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="E86" t="s">
-        <v>319</v>
-      </c>
-      <c r="F86" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" ht="21">
-      <c r="A87" t="s">
-        <v>324</v>
-      </c>
-      <c r="B87">
-        <v>0</v>
-      </c>
       <c r="C87" s="1" t="s">
-        <v>322</v>
+        <v>85</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>325</v>
+        <v>94</v>
       </c>
       <c r="E87" t="s">
-        <v>319</v>
+        <v>70</v>
       </c>
       <c r="F87" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" ht="63">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" ht="42">
+      <c r="A88" t="s">
+        <v>78</v>
+      </c>
       <c r="B88">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>323</v>
+        <v>86</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="E88" t="s">
-        <v>319</v>
+        <v>70</v>
       </c>
       <c r="F88" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" ht="63">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" ht="42">
       <c r="A89" t="s">
-        <v>119</v>
+        <v>78</v>
       </c>
       <c r="B89">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>118</v>
+        <v>87</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>120</v>
+        <v>95</v>
       </c>
       <c r="E89" t="s">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="F89" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" ht="105">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" ht="42">
       <c r="A90" t="s">
-        <v>209</v>
+        <v>78</v>
       </c>
       <c r="B90">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>205</v>
+        <v>88</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>5</v>
+        <v>96</v>
       </c>
       <c r="E90" t="s">
-        <v>311</v>
+        <v>70</v>
       </c>
       <c r="F90" t="s">
-        <v>206</v>
-      </c>
-      <c r="H90" s="4" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8" ht="21">
-      <c r="A91" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" ht="42">
+      <c r="A91" t="s">
+        <v>78</v>
       </c>
       <c r="B91">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>33</v>
+        <v>89</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>35</v>
+        <v>97</v>
       </c>
       <c r="E91" t="s">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="F91" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" ht="84">
-      <c r="A92" s="2" t="s">
-        <v>31</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" ht="168">
+      <c r="A92" t="s">
+        <v>78</v>
       </c>
       <c r="B92">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>32</v>
+        <v>90</v>
       </c>
       <c r="D92" s="1" t="s">
         <v>5</v>
@@ -8248,41 +8680,41 @@
         <v>45</v>
       </c>
       <c r="F92" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" ht="336">
-      <c r="A93" s="2" t="s">
-        <v>27</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" ht="42">
+      <c r="A93" t="s">
+        <v>78</v>
       </c>
       <c r="B93">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>28</v>
+        <v>91</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E93" t="s">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="F93" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="94" spans="1:8" ht="63">
-      <c r="A94" s="2" t="s">
-        <v>27</v>
+    <row r="94" spans="1:7" ht="42">
+      <c r="A94" t="s">
+        <v>99</v>
       </c>
       <c r="B94">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>29</v>
+        <v>98</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>5</v>
+        <v>104</v>
       </c>
       <c r="E94" t="s">
         <v>45</v>
@@ -8291,15 +8723,15 @@
         <v>39</v>
       </c>
     </row>
-    <row r="95" spans="1:8" ht="63">
+    <row r="95" spans="1:7" ht="42">
       <c r="A95" t="s">
-        <v>12</v>
+        <v>100</v>
       </c>
       <c r="B95">
         <v>0</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>13</v>
+        <v>101</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>5</v>
@@ -8308,38 +8740,38 @@
         <v>45</v>
       </c>
       <c r="F95" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8" ht="63">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" ht="84">
       <c r="A96" t="s">
-        <v>12</v>
+        <v>103</v>
       </c>
       <c r="B96">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>14</v>
+        <v>369</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>5</v>
+        <v>105</v>
       </c>
       <c r="E96" t="s">
-        <v>45</v>
+        <v>309</v>
       </c>
       <c r="F96" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="97" spans="1:8" ht="63">
       <c r="A97" t="s">
-        <v>11</v>
+        <v>106</v>
       </c>
       <c r="B97">
         <v>0</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>10</v>
+        <v>107</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>5</v>
@@ -8351,38 +8783,35 @@
         <v>39</v>
       </c>
     </row>
-    <row r="98" spans="1:8" ht="84">
+    <row r="98" spans="1:8" ht="126">
       <c r="A98" t="s">
-        <v>176</v>
+        <v>108</v>
       </c>
       <c r="B98">
         <v>0</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>177</v>
+        <v>109</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>5</v>
+        <v>110</v>
       </c>
       <c r="E98" t="s">
-        <v>178</v>
+        <v>45</v>
       </c>
       <c r="F98" t="s">
         <v>46</v>
       </c>
-      <c r="H98" s="4" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8" ht="63">
+    </row>
+    <row r="99" spans="1:8" ht="42">
       <c r="A99" t="s">
-        <v>7</v>
+        <v>108</v>
       </c>
       <c r="B99">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="D99" s="1" t="s">
         <v>5</v>
@@ -8391,227 +8820,221 @@
         <v>45</v>
       </c>
       <c r="F99" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="100" spans="1:8" ht="105">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" ht="147">
       <c r="A100" t="s">
-        <v>6</v>
+        <v>112</v>
       </c>
       <c r="B100">
         <v>0</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>4</v>
+        <v>113</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>5</v>
+        <v>114</v>
       </c>
       <c r="E100" t="s">
         <v>45</v>
       </c>
       <c r="F100" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
     </row>
     <row r="101" spans="1:8" ht="105">
       <c r="A101" t="s">
-        <v>71</v>
+        <v>115</v>
       </c>
       <c r="B101">
         <v>0</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>72</v>
+        <v>116</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>65</v>
+        <v>5</v>
       </c>
       <c r="E101" t="s">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="F101" t="s">
-        <v>66</v>
+        <v>39</v>
       </c>
     </row>
     <row r="102" spans="1:8" ht="42">
       <c r="A102" t="s">
-        <v>67</v>
+        <v>295</v>
       </c>
       <c r="B102">
         <v>0</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>68</v>
+        <v>294</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>69</v>
+        <v>5</v>
       </c>
       <c r="E102" t="s">
-        <v>70</v>
+        <v>296</v>
       </c>
       <c r="F102" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="103" spans="1:8" ht="84">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" ht="42">
       <c r="A103" t="s">
-        <v>174</v>
+        <v>316</v>
       </c>
       <c r="B103">
         <v>0</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="D103" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="E103" s="6" t="s">
-        <v>310</v>
-      </c>
-      <c r="F103" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="H103" s="4" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8" ht="42">
+        <v>317</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="E103" t="s">
+        <v>318</v>
+      </c>
+      <c r="F103" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" ht="21">
       <c r="A104" t="s">
-        <v>64</v>
+        <v>323</v>
       </c>
       <c r="B104">
         <v>0</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>77</v>
+        <v>321</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>65</v>
+        <v>324</v>
       </c>
       <c r="E104" t="s">
-        <v>45</v>
+        <v>318</v>
       </c>
       <c r="F104" t="s">
-        <v>66</v>
+        <v>280</v>
       </c>
     </row>
     <row r="105" spans="1:8" ht="63">
-      <c r="A105" t="s">
-        <v>62</v>
-      </c>
       <c r="B105">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>60</v>
+        <v>322</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
       <c r="E105" t="s">
-        <v>45</v>
+        <v>318</v>
       </c>
       <c r="F105" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="106" spans="1:8" ht="126">
-      <c r="A106" s="2" t="s">
-        <v>42</v>
+        <v>325</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" ht="63">
+      <c r="A106" t="s">
+        <v>118</v>
       </c>
       <c r="B106">
         <v>0</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>43</v>
+        <v>117</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>44</v>
+        <v>119</v>
       </c>
       <c r="E106" t="s">
-        <v>224</v>
+        <v>45</v>
       </c>
       <c r="F106" t="s">
         <v>46</v>
       </c>
-      <c r="G106" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8" ht="21">
-      <c r="A107" s="2" t="s">
-        <v>15</v>
+    </row>
+    <row r="107" spans="1:8" ht="105">
+      <c r="A107" t="s">
+        <v>208</v>
       </c>
       <c r="B107">
         <v>0</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>16</v>
+        <v>204</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="E107" t="s">
-        <v>45</v>
+        <v>310</v>
       </c>
       <c r="F107" t="s">
-        <v>36</v>
+        <v>205</v>
+      </c>
+      <c r="H107" s="4" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="108" spans="1:8" ht="21">
       <c r="A108" s="2" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="B108">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="E108" t="s">
         <v>45</v>
       </c>
       <c r="F108" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8" ht="42">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" ht="84">
       <c r="A109" s="2" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="B109">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="E109" t="s">
         <v>45</v>
       </c>
       <c r="F109" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8" ht="21">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" ht="336">
       <c r="A110" s="2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="B110">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>74</v>
+        <v>28</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="E110" t="s">
         <v>45</v>
@@ -8620,396 +9043,746 @@
         <v>36</v>
       </c>
     </row>
-    <row r="111" spans="1:8" ht="42">
+    <row r="111" spans="1:8" ht="63">
       <c r="A111" s="2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="B111">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>73</v>
+        <v>29</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="E111" t="s">
         <v>45</v>
       </c>
       <c r="F111" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="112" spans="1:8" ht="21">
-      <c r="A112" s="2" t="s">
-        <v>15</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" ht="63">
+      <c r="A112" t="s">
+        <v>12</v>
       </c>
       <c r="B112">
+        <v>0</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D112" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="C112" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D112" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="E112" t="s">
         <v>45</v>
       </c>
       <c r="F112" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="113" spans="1:8" ht="21">
-      <c r="A113" s="2" t="s">
-        <v>15</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" ht="63">
+      <c r="A113" t="s">
+        <v>12</v>
       </c>
       <c r="B113">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>76</v>
+        <v>14</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="E113" t="s">
         <v>45</v>
       </c>
       <c r="F113" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="114" spans="1:8" ht="21">
-      <c r="A114" s="2" t="s">
-        <v>15</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" ht="63">
+      <c r="A114" t="s">
+        <v>11</v>
       </c>
       <c r="B114">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="E114" t="s">
         <v>45</v>
       </c>
       <c r="F114" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="115" spans="1:8" ht="21">
-      <c r="A115" s="2" t="s">
-        <v>170</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" ht="84">
+      <c r="A115" t="s">
+        <v>175</v>
       </c>
       <c r="B115">
         <v>0</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="D115" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E115" t="s">
-        <v>45</v>
+        <v>177</v>
       </c>
       <c r="F115" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="H115" s="4" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="116" spans="1:8" ht="409.6">
-      <c r="A116" s="2" t="s">
-        <v>170</v>
+        <v>161</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" ht="63">
+      <c r="A116" t="s">
+        <v>7</v>
       </c>
       <c r="B116">
-        <v>1</v>
-      </c>
-      <c r="C116" s="3" t="s">
-        <v>172</v>
+        <v>0</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E116" t="s">
-        <v>225</v>
+        <v>45</v>
       </c>
       <c r="F116" t="s">
-        <v>36</v>
-      </c>
-      <c r="H116" s="4"/>
+        <v>37</v>
+      </c>
     </row>
     <row r="117" spans="1:8" ht="105">
-      <c r="A117" s="2" t="s">
-        <v>63</v>
+      <c r="A117" t="s">
+        <v>6</v>
       </c>
       <c r="B117">
         <v>0</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>59</v>
+        <v>4</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>160</v>
+        <v>5</v>
       </c>
       <c r="E117" t="s">
         <v>45</v>
       </c>
       <c r="F117" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="118" spans="1:8" ht="63">
-      <c r="A118" s="2" t="s">
-        <v>58</v>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" ht="105">
+      <c r="A118" t="s">
+        <v>71</v>
       </c>
       <c r="B118">
         <v>0</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>5</v>
+        <v>65</v>
       </c>
       <c r="E118" t="s">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="F118" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
     </row>
     <row r="119" spans="1:8" ht="42">
-      <c r="A119" s="2" t="s">
-        <v>56</v>
+      <c r="A119" t="s">
+        <v>67</v>
       </c>
       <c r="B119">
         <v>0</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>5</v>
+        <v>69</v>
       </c>
       <c r="E119" t="s">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="F119" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="120" spans="1:8" ht="21">
-      <c r="A120" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" ht="84">
+      <c r="A120" t="s">
+        <v>173</v>
       </c>
       <c r="B120">
         <v>0</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D120" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E120" t="s">
-        <v>45</v>
-      </c>
-      <c r="F120" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="121" spans="1:8" ht="84">
-      <c r="A121" s="2" t="s">
-        <v>51</v>
+        <v>174</v>
+      </c>
+      <c r="D120" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="E120" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="F120" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="H120" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" ht="42">
+      <c r="A121" t="s">
+        <v>64</v>
       </c>
       <c r="B121">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>5</v>
+        <v>65</v>
       </c>
       <c r="E121" t="s">
         <v>45</v>
       </c>
       <c r="F121" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="122" spans="1:8" ht="42">
-      <c r="A122" s="2" t="s">
-        <v>47</v>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" ht="63">
+      <c r="A122" t="s">
+        <v>62</v>
       </c>
       <c r="B122">
         <v>0</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>161</v>
+        <v>61</v>
       </c>
       <c r="E122" t="s">
         <v>45</v>
       </c>
       <c r="F122" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="123" spans="1:8" ht="42">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" ht="126">
       <c r="A123" s="2" t="s">
-        <v>166</v>
+        <v>42</v>
       </c>
       <c r="B123">
         <v>0</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>165</v>
+        <v>43</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>167</v>
+        <v>44</v>
       </c>
       <c r="E123" t="s">
-        <v>168</v>
+        <v>223</v>
       </c>
       <c r="F123" t="s">
-        <v>169</v>
-      </c>
-      <c r="H123" s="4" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="124" spans="1:8" ht="126">
+        <v>46</v>
+      </c>
+      <c r="G123" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" ht="21">
       <c r="A124" s="2" t="s">
-        <v>163</v>
+        <v>15</v>
       </c>
       <c r="B124">
         <v>0</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>164</v>
+        <v>16</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="E124" t="s">
-        <v>226</v>
+        <v>45</v>
       </c>
       <c r="F124" t="s">
-        <v>299</v>
-      </c>
-      <c r="H124" s="4" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="125" spans="1:8" ht="105">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" ht="21">
       <c r="A125" s="2" t="s">
-        <v>157</v>
+        <v>15</v>
       </c>
       <c r="B125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="E125" t="s">
-        <v>313</v>
+        <v>45</v>
       </c>
       <c r="F125" t="s">
-        <v>299</v>
-      </c>
-      <c r="H125" s="4" t="s">
-        <v>162</v>
+        <v>36</v>
       </c>
     </row>
     <row r="126" spans="1:8" ht="42">
       <c r="A126" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B126">
+        <v>2</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E126" t="s">
+        <v>45</v>
+      </c>
+      <c r="F126" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" ht="21">
+      <c r="A127" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B127">
+        <v>3</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E127" t="s">
+        <v>45</v>
+      </c>
+      <c r="F127" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" ht="42">
+      <c r="A128" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B128">
+        <v>4</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D128" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E128" t="s">
+        <v>45</v>
+      </c>
+      <c r="F128" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" ht="21">
+      <c r="A129" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B129">
+        <v>5</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E129" t="s">
+        <v>45</v>
+      </c>
+      <c r="F129" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" ht="21">
+      <c r="A130" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B130">
+        <v>6</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E130" t="s">
+        <v>45</v>
+      </c>
+      <c r="F130" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" ht="21">
+      <c r="A131" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B131">
+        <v>7</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E131" t="s">
+        <v>45</v>
+      </c>
+      <c r="F131" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" ht="21">
+      <c r="A132" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B132">
+        <v>0</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D132" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E132" t="s">
+        <v>45</v>
+      </c>
+      <c r="F132" t="s">
+        <v>36</v>
+      </c>
+      <c r="H132" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" ht="409.6">
+      <c r="A133" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B133">
+        <v>1</v>
+      </c>
+      <c r="C133" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D133" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E133" t="s">
+        <v>224</v>
+      </c>
+      <c r="F133" t="s">
+        <v>36</v>
+      </c>
+      <c r="H133" s="4"/>
+    </row>
+    <row r="134" spans="1:8" ht="105">
+      <c r="A134" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B134">
+        <v>0</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D134" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E134" t="s">
+        <v>45</v>
+      </c>
+      <c r="F134" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" ht="63">
+      <c r="A135" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B135">
+        <v>0</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D135" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E135" t="s">
+        <v>45</v>
+      </c>
+      <c r="F135" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" ht="42">
+      <c r="A136" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B136">
+        <v>0</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D136" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E136" t="s">
+        <v>45</v>
+      </c>
+      <c r="F136" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" ht="21">
+      <c r="A137" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B137">
+        <v>0</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D137" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E137" t="s">
+        <v>45</v>
+      </c>
+      <c r="F137" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" ht="84">
+      <c r="A138" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B138">
+        <v>1</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D138" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E138" t="s">
+        <v>45</v>
+      </c>
+      <c r="F138" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" ht="42">
+      <c r="A139" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B139">
+        <v>0</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D139" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E139" t="s">
+        <v>45</v>
+      </c>
+      <c r="F139" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" ht="42">
+      <c r="A140" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B140">
+        <v>0</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D140" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E140" t="s">
+        <v>167</v>
+      </c>
+      <c r="F140" t="s">
+        <v>168</v>
+      </c>
+      <c r="H140" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" ht="126">
+      <c r="A141" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B141">
+        <v>0</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D141" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E141" t="s">
+        <v>225</v>
+      </c>
+      <c r="F141" t="s">
+        <v>298</v>
+      </c>
+      <c r="H141" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" ht="105">
+      <c r="A142" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B142">
+        <v>0</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D142" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E142" t="s">
+        <v>312</v>
+      </c>
+      <c r="F142" t="s">
+        <v>298</v>
+      </c>
+      <c r="H142" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" ht="42">
+      <c r="A143" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B143">
+        <v>1</v>
+      </c>
+      <c r="C143" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="B126">
-        <v>1</v>
-      </c>
-      <c r="C126" s="1" t="s">
+      <c r="D143" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="D126" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="E126" t="s">
+      <c r="E143" t="s">
         <v>70</v>
       </c>
-      <c r="F126" t="s">
-        <v>299</v>
-      </c>
-      <c r="H126" s="4"/>
-    </row>
-    <row r="127" spans="1:8" ht="42">
-      <c r="A127" s="2" t="s">
+      <c r="F143" t="s">
+        <v>298</v>
+      </c>
+      <c r="H143" s="4"/>
+    </row>
+    <row r="144" spans="1:8" ht="42">
+      <c r="A144" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B144">
+        <v>0</v>
+      </c>
+      <c r="C144" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B127">
-        <v>0</v>
-      </c>
-      <c r="C127" s="1" t="s">
+      <c r="D144" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E144" t="s">
         <v>154</v>
       </c>
-      <c r="D127" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E127" t="s">
-        <v>155</v>
-      </c>
-      <c r="F127" t="s">
+      <c r="F144" t="s">
         <v>40</v>
       </c>
-      <c r="H127" s="4" t="s">
-        <v>162</v>
+      <c r="H144" s="4" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <hyperlinks>
-    <hyperlink ref="H127" r:id="rId1" xr:uid="{81642C6C-B155-384F-AAC7-449D3395E8A1}"/>
-    <hyperlink ref="H125" r:id="rId2" xr:uid="{BF840327-7DE3-494E-9852-F70E198FA83F}"/>
-    <hyperlink ref="H124" r:id="rId3" xr:uid="{C1032CAE-FCD8-1242-B6C3-B70B988BC2CA}"/>
-    <hyperlink ref="H123" r:id="rId4" xr:uid="{F8DE77CC-7236-5740-A008-5EFF79B59035}"/>
-    <hyperlink ref="H115" r:id="rId5" xr:uid="{09EF007C-85D3-5F45-B203-6FE0424E5C99}"/>
-    <hyperlink ref="H103" r:id="rId6" xr:uid="{CA79A61E-3453-F748-8421-4D89662469BF}"/>
-    <hyperlink ref="H98" r:id="rId7" xr:uid="{DF2D3758-0BC9-D246-BED3-26AF94D5F9D8}"/>
-    <hyperlink ref="H50" r:id="rId8" xr:uid="{CCDC15F7-E252-0348-B02C-905084BD776E}"/>
-    <hyperlink ref="H13" r:id="rId9" xr:uid="{B4649428-221F-674F-BA70-A2780E5E269C}"/>
-    <hyperlink ref="H90" r:id="rId10" xr:uid="{E8486F26-D2AA-3540-A8B3-73E08A241E3A}"/>
-    <hyperlink ref="H20" r:id="rId11" xr:uid="{DF9E283C-C630-6141-B84A-D4DC20067D3A}"/>
-    <hyperlink ref="H21" r:id="rId12" xr:uid="{AA765222-2C31-E444-93E0-6241B574BBDA}"/>
-    <hyperlink ref="H24" r:id="rId13" xr:uid="{7424A509-2E7F-534F-A182-16DD568A0E14}"/>
-    <hyperlink ref="H26" r:id="rId14" xr:uid="{B81B5BB0-A4D2-CE48-976B-41038463380C}"/>
-    <hyperlink ref="H27" r:id="rId15" xr:uid="{51731D61-79A9-C248-A29C-7F455B171752}"/>
-    <hyperlink ref="H28" r:id="rId16" xr:uid="{DF071ACD-52CF-F248-82F5-DCBA80F5ED7C}"/>
-    <hyperlink ref="H29" r:id="rId17" xr:uid="{A3CDB931-1A52-EE43-BE32-2575167D2188}"/>
-    <hyperlink ref="H31" r:id="rId18" xr:uid="{217C257E-AC48-D240-A20A-4B4B59D80A75}"/>
-    <hyperlink ref="H32" r:id="rId19" xr:uid="{7DD8D092-ADED-CC44-8C91-A6B96A4E7F8B}"/>
-    <hyperlink ref="H33" r:id="rId20" xr:uid="{FF12F444-682A-3040-A650-0D77B1F409BF}"/>
-    <hyperlink ref="H34" r:id="rId21" xr:uid="{1128B72D-52B8-8F47-9418-E2DF8EDBE41D}"/>
-    <hyperlink ref="H43" r:id="rId22" xr:uid="{497C3D62-66B1-B349-919C-BB1436BCE7EA}"/>
-    <hyperlink ref="H49" r:id="rId23" xr:uid="{AA737391-1EFB-A246-BB33-46BEF9DF59DA}"/>
-    <hyperlink ref="H47" r:id="rId24" xr:uid="{12373DBC-12D0-EF44-94D1-6BE389EE8541}"/>
-    <hyperlink ref="H46" r:id="rId25" xr:uid="{0D1FF725-B522-814B-944C-9DE55388698D}"/>
-    <hyperlink ref="H48" r:id="rId26" xr:uid="{B196E238-6A79-1D4C-BE62-208D54322587}"/>
-    <hyperlink ref="H44" r:id="rId27" xr:uid="{C086B470-F6CB-A541-BF4F-D4066F6C3477}"/>
-    <hyperlink ref="H45" r:id="rId28" xr:uid="{6C629B57-C1F3-4545-97A0-DAE1AEC86284}"/>
-    <hyperlink ref="H42" r:id="rId29" xr:uid="{B29892C6-C28D-A544-98D7-253097387448}"/>
-    <hyperlink ref="H41" r:id="rId30" xr:uid="{CB97C88D-610F-9244-AD06-BA36E3E1A20C}"/>
+    <hyperlink ref="H144" r:id="rId1" xr:uid="{81642C6C-B155-384F-AAC7-449D3395E8A1}"/>
+    <hyperlink ref="H142" r:id="rId2" xr:uid="{BF840327-7DE3-494E-9852-F70E198FA83F}"/>
+    <hyperlink ref="H141" r:id="rId3" xr:uid="{C1032CAE-FCD8-1242-B6C3-B70B988BC2CA}"/>
+    <hyperlink ref="H140" r:id="rId4" xr:uid="{F8DE77CC-7236-5740-A008-5EFF79B59035}"/>
+    <hyperlink ref="H132" r:id="rId5" xr:uid="{09EF007C-85D3-5F45-B203-6FE0424E5C99}"/>
+    <hyperlink ref="H120" r:id="rId6" xr:uid="{CA79A61E-3453-F748-8421-4D89662469BF}"/>
+    <hyperlink ref="H115" r:id="rId7" xr:uid="{DF2D3758-0BC9-D246-BED3-26AF94D5F9D8}"/>
+    <hyperlink ref="H67" r:id="rId8" xr:uid="{CCDC15F7-E252-0348-B02C-905084BD776E}"/>
+    <hyperlink ref="H30" r:id="rId9" xr:uid="{B4649428-221F-674F-BA70-A2780E5E269C}"/>
+    <hyperlink ref="H107" r:id="rId10" xr:uid="{E8486F26-D2AA-3540-A8B3-73E08A241E3A}"/>
+    <hyperlink ref="H37" r:id="rId11" xr:uid="{DF9E283C-C630-6141-B84A-D4DC20067D3A}"/>
+    <hyperlink ref="H38" r:id="rId12" xr:uid="{AA765222-2C31-E444-93E0-6241B574BBDA}"/>
+    <hyperlink ref="H41" r:id="rId13" xr:uid="{7424A509-2E7F-534F-A182-16DD568A0E14}"/>
+    <hyperlink ref="H43" r:id="rId14" xr:uid="{B81B5BB0-A4D2-CE48-976B-41038463380C}"/>
+    <hyperlink ref="H44" r:id="rId15" xr:uid="{51731D61-79A9-C248-A29C-7F455B171752}"/>
+    <hyperlink ref="H45" r:id="rId16" xr:uid="{DF071ACD-52CF-F248-82F5-DCBA80F5ED7C}"/>
+    <hyperlink ref="H46" r:id="rId17" xr:uid="{A3CDB931-1A52-EE43-BE32-2575167D2188}"/>
+    <hyperlink ref="H48" r:id="rId18" xr:uid="{217C257E-AC48-D240-A20A-4B4B59D80A75}"/>
+    <hyperlink ref="H49" r:id="rId19" xr:uid="{7DD8D092-ADED-CC44-8C91-A6B96A4E7F8B}"/>
+    <hyperlink ref="H50" r:id="rId20" xr:uid="{FF12F444-682A-3040-A650-0D77B1F409BF}"/>
+    <hyperlink ref="H51" r:id="rId21" xr:uid="{1128B72D-52B8-8F47-9418-E2DF8EDBE41D}"/>
+    <hyperlink ref="H60" r:id="rId22" xr:uid="{497C3D62-66B1-B349-919C-BB1436BCE7EA}"/>
+    <hyperlink ref="H66" r:id="rId23" xr:uid="{AA737391-1EFB-A246-BB33-46BEF9DF59DA}"/>
+    <hyperlink ref="H64" r:id="rId24" xr:uid="{12373DBC-12D0-EF44-94D1-6BE389EE8541}"/>
+    <hyperlink ref="H63" r:id="rId25" xr:uid="{0D1FF725-B522-814B-944C-9DE55388698D}"/>
+    <hyperlink ref="H65" r:id="rId26" xr:uid="{B196E238-6A79-1D4C-BE62-208D54322587}"/>
+    <hyperlink ref="H61" r:id="rId27" xr:uid="{C086B470-F6CB-A541-BF4F-D4066F6C3477}"/>
+    <hyperlink ref="H62" r:id="rId28" xr:uid="{6C629B57-C1F3-4545-97A0-DAE1AEC86284}"/>
+    <hyperlink ref="H59" r:id="rId29" xr:uid="{B29892C6-C28D-A544-98D7-253097387448}"/>
+    <hyperlink ref="H58" r:id="rId30" xr:uid="{CB97C88D-610F-9244-AD06-BA36E3E1A20C}"/>
+    <hyperlink ref="H16" r:id="rId31" xr:uid="{E92164C8-75EB-FE45-8332-C3A91BA4451A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
fix typo in data
</commit_message>
<xml_diff>
--- a/data_excel/tags.xlsx
+++ b/data_excel/tags.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jay/xidev/kanban/data_excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{65083B93-1A1A-7D4F-966A-166A6837CE95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{3F49C4DB-6B55-CC46-861A-C6ABCDBDD7D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16940" yWindow="660" windowWidth="21300" windowHeight="17120" xr2:uid="{1951D371-7A8D-D346-B651-736256765602}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="408">
   <si>
     <t>img</t>
     <phoneticPr fontId="1"/>
@@ -5225,9 +5225,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>IMG_1663.HEIC</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">芝生内に入らないでください
 Please do not walk on the lawn.
@@ -6188,6 +6185,17 @@
   </si>
   <si>
     <t>IMG_1161.jpg</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>大和西大寺</t>
+    <rPh sb="0" eb="1">
+      <t>ヤマトサ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>IMG_1671.HEIC</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -6698,8 +6706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0244D4E8-F443-D54E-A975-960F8853E327}">
   <dimension ref="A1:H144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="106" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="106" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -6758,7 +6766,7 @@
         <v>333</v>
       </c>
       <c r="G2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="84">
@@ -6781,7 +6789,7 @@
         <v>337</v>
       </c>
       <c r="G3" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="126">
@@ -6804,7 +6812,7 @@
         <v>46</v>
       </c>
       <c r="G4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="147">
@@ -6827,7 +6835,7 @@
         <v>40</v>
       </c>
       <c r="G5" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="147">
@@ -6850,18 +6858,18 @@
         <v>40</v>
       </c>
       <c r="G6" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="147">
       <c r="A7" t="s">
-        <v>346</v>
+        <v>407</v>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>5</v>
@@ -6873,21 +6881,21 @@
         <v>39</v>
       </c>
       <c r="G7" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="147">
       <c r="A8" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B8">
         <v>0</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>349</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>350</v>
       </c>
       <c r="E8" t="s">
         <v>345</v>
@@ -6896,41 +6904,41 @@
         <v>40</v>
       </c>
       <c r="G8" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="147">
       <c r="A9" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B9">
         <v>0</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E9" t="s">
         <v>345</v>
       </c>
       <c r="F9" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G9" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="147">
       <c r="A10" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B10">
         <v>0</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>5</v>
@@ -6942,21 +6950,21 @@
         <v>36</v>
       </c>
       <c r="G10" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="63">
       <c r="A11" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B11">
         <v>0</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>363</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>364</v>
       </c>
       <c r="E11" t="s">
         <v>45</v>
@@ -6965,18 +6973,18 @@
         <v>298</v>
       </c>
       <c r="G11" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="21">
       <c r="A12" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B12">
         <v>0</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>5</v>
@@ -6985,24 +6993,24 @@
         <v>45</v>
       </c>
       <c r="F12" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="G12" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="42">
       <c r="A13" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B13">
         <v>0</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>379</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>380</v>
       </c>
       <c r="E13" t="s">
         <v>45</v>
@@ -7013,16 +7021,16 @@
     </row>
     <row r="14" spans="1:8" ht="126">
       <c r="A14" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B14">
         <v>0</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>381</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>382</v>
       </c>
       <c r="E14" t="s">
         <v>45</v>
@@ -7031,21 +7039,21 @@
         <v>36</v>
       </c>
       <c r="G14" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="42">
       <c r="A15" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B15">
         <v>0</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>384</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>385</v>
       </c>
       <c r="E15" t="s">
         <v>70</v>
@@ -7054,21 +7062,21 @@
         <v>36</v>
       </c>
       <c r="G15" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="42">
       <c r="A16" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B16">
         <v>0</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>387</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>388</v>
       </c>
       <c r="E16" t="s">
         <v>200</v>
@@ -7077,21 +7085,21 @@
         <v>39</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="105">
       <c r="A17" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B17">
         <v>0</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E17" t="s">
         <v>45</v>
@@ -7102,13 +7110,13 @@
     </row>
     <row r="18" spans="1:8" ht="63">
       <c r="A18" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B18">
         <v>0</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>5</v>
@@ -7122,119 +7130,122 @@
     </row>
     <row r="19" spans="1:8" ht="21">
       <c r="A19" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B19">
         <v>0</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="E19" t="s">
+        <v>392</v>
+      </c>
+      <c r="F19" t="s">
         <v>393</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>396</v>
-      </c>
-      <c r="E19" t="s">
-        <v>393</v>
-      </c>
-      <c r="F19" t="s">
-        <v>394</v>
+      <c r="G19" t="s">
+        <v>406</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="21">
       <c r="A20" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="E20" t="s">
+        <v>392</v>
+      </c>
+      <c r="F20" t="s">
         <v>393</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>397</v>
-      </c>
-      <c r="E20" t="s">
-        <v>393</v>
-      </c>
-      <c r="F20" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="21">
       <c r="A21" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B21">
         <v>2</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="E21" t="s">
+        <v>392</v>
+      </c>
+      <c r="F21" t="s">
         <v>393</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="E21" t="s">
-        <v>393</v>
-      </c>
-      <c r="F21" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="21">
       <c r="A22" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B22">
         <v>3</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="E22" t="s">
+        <v>392</v>
+      </c>
+      <c r="F22" t="s">
         <v>393</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>398</v>
-      </c>
-      <c r="E22" t="s">
-        <v>393</v>
-      </c>
-      <c r="F22" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="21">
       <c r="A23" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B23">
         <v>4</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="E23" t="s">
+        <v>392</v>
+      </c>
+      <c r="F23" t="s">
         <v>393</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="E23" t="s">
-        <v>393</v>
-      </c>
-      <c r="F23" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="21">
       <c r="A24" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B24">
         <v>0</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E24" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F24" t="s">
         <v>280</v>
@@ -7242,19 +7253,19 @@
     </row>
     <row r="25" spans="1:8" ht="21">
       <c r="A25" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B25">
         <v>1</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E25" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F25" t="s">
         <v>280</v>
@@ -7262,19 +7273,19 @@
     </row>
     <row r="26" spans="1:8" ht="21">
       <c r="A26" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B26">
         <v>2</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E26" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F26" t="s">
         <v>280</v>
@@ -7282,19 +7293,19 @@
     </row>
     <row r="27" spans="1:8" ht="21">
       <c r="A27" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B27">
         <v>3</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="E27" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F27" t="s">
         <v>280</v>
@@ -7302,42 +7313,42 @@
     </row>
     <row r="28" spans="1:8" ht="21">
       <c r="A28" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B28">
         <v>0</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E28" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F28" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="21">
       <c r="A29" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
       <c r="C29" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>403</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>404</v>
       </c>
       <c r="E29" t="s">
         <v>45</v>
       </c>
       <c r="F29" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="147">
@@ -7392,7 +7403,7 @@
         <v>0</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>282</v>
@@ -8480,7 +8491,7 @@
         <v>36</v>
       </c>
       <c r="G82" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="84">
@@ -8751,7 +8762,7 @@
         <v>0</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>105</v>
@@ -9309,7 +9320,7 @@
         <v>46</v>
       </c>
       <c r="G123" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="124" spans="1:8" ht="21">

</xml_diff>